<commit_message>
Reducing some confusion and duplication by eliminating separate "trimmed_database" files; moved trimmed acylRanges table to new tab in .xlsx file and ported over the .csv
</commit_message>
<xml_diff>
--- a/inst/doc/default_database/xlsx/LOBSTAHS_acylRanges.xlsx
+++ b/inst/doc/default_database/xlsx/LOBSTAHS_acylRanges.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/LOBSTAHS/inst/doc/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/default_database/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D44346-F236-9E4F-8A23-57A2EF80937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="39100" yWindow="3280" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_acylRanges" sheetId="5" r:id="rId1"/>
-    <sheet name="Notes" sheetId="4" r:id="rId2"/>
+    <sheet name="LOBSTAHS_acylRanges_trimmed" sheetId="6" r:id="rId2"/>
+    <sheet name="Notes" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Provided under an Apache 2.0 license; attribution required</t>
   </si>
@@ -115,12 +117,18 @@
   </si>
   <si>
     <t>Navigate to the worksheet "LOBSTAHS_acylRanges", then export as a .csv with the filename "LOBSTAHS_acylRanges.csv"; this file can be sourced by specifying the file path in the LOBSTAHS database generation function generateLOBdbase()</t>
+  </si>
+  <si>
+    <t>Added an alternate acylRanges table ("LOBSTAHS_acylRanges_trimmed") that will generate a reduced database of species with a narrower range of acyl chain lengths; for use in the Van Mooy Lab</t>
+  </si>
+  <si>
+    <t>TL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -267,6 +275,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -593,11 +604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1769,11 +1780,752 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8EBD5A-DBD2-D542-8576-9FF874ACB2F6}">
+  <dimension ref="A1:K66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>45</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>46</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>47</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>48</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>49</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>51</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>53</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>54</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>55</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>56</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>57</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>58</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1882,6 +2634,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>43025</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>